<commit_message>
Removed unused analyses and removed side-scoring
</commit_message>
<xml_diff>
--- a/outputs/descriptives.xlsx
+++ b/outputs/descriptives.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24026"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24131"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\py\gsa\outputs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{80DA9DDF-D37F-4844-AAED-B87753924BC9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{39B31172-5F2D-42A1-ADC8-EA121E714C2B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="38280" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="39210" yWindow="-120" windowWidth="28110" windowHeight="16440" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="descriptives" sheetId="1" r:id="rId1"/>
@@ -109,9 +109,6 @@
     <t>Game</t>
   </si>
   <si>
-    <t>Interactive visualisation</t>
-  </si>
-  <si>
     <t>MCQ score</t>
   </si>
   <si>
@@ -128,6 +125,9 @@
   </si>
   <si>
     <t>Control</t>
+  </si>
+  <si>
+    <t>Non-game</t>
   </si>
 </sst>
 </file>
@@ -614,11 +614,12 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -769,7 +770,7 @@
           </c:tx>
           <c:spPr>
             <a:solidFill>
-              <a:schemeClr val="accent1"/>
+              <a:schemeClr val="tx1"/>
             </a:solidFill>
             <a:ln>
               <a:noFill/>
@@ -825,7 +826,7 @@
             <c:numRef>
               <c:f>PLEX!$B$2:$B$13</c:f>
               <c:numCache>
-                <c:formatCode>0.0</c:formatCode>
+                <c:formatCode>0%</c:formatCode>
                 <c:ptCount val="12"/>
                 <c:pt idx="0">
                   <c:v>0.64444444444444404</c:v>
@@ -881,7 +882,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>Interactive visualisation</c:v>
+                  <c:v>Non-game</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -944,7 +945,7 @@
             <c:numRef>
               <c:f>PLEX!$C$2:$C$13</c:f>
               <c:numCache>
-                <c:formatCode>0.0</c:formatCode>
+                <c:formatCode>0%</c:formatCode>
                 <c:ptCount val="12"/>
                 <c:pt idx="0">
                   <c:v>0.152941176470588</c:v>
@@ -1060,6 +1061,7 @@
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="1"/>
+          <c:min val="0"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="l"/>
@@ -1077,7 +1079,7 @@
             <a:effectLst/>
           </c:spPr>
         </c:majorGridlines>
-        <c:numFmt formatCode="0.0" sourceLinked="1"/>
+        <c:numFmt formatCode="0%" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
@@ -1111,7 +1113,7 @@
         <c:crossAx val="819298192"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
-        <c:majorUnit val="0.2"/>
+        <c:majorUnit val="0.25"/>
       </c:valAx>
       <c:spPr>
         <a:noFill/>
@@ -1161,12 +1163,7 @@
       <a:schemeClr val="bg1"/>
     </a:solidFill>
     <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-      <a:solidFill>
-        <a:schemeClr val="tx1">
-          <a:lumMod val="15000"/>
-          <a:lumOff val="85000"/>
-        </a:schemeClr>
-      </a:solidFill>
+      <a:noFill/>
       <a:round/>
     </a:ln>
     <a:effectLst/>
@@ -2073,7 +2070,7 @@
   <dimension ref="A1:F23"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A5" sqref="A5:A20"/>
+      <selection activeCell="A24" sqref="A24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2100,7 +2097,7 @@
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B2">
         <v>175</v>
@@ -2160,7 +2157,7 @@
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B5">
         <v>175</v>
@@ -2420,7 +2417,7 @@
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B18">
         <v>175</v>
@@ -2440,7 +2437,7 @@
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B19">
         <v>175</v>
@@ -2460,7 +2457,7 @@
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B20">
         <v>175</v>
@@ -2499,7 +2496,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E4A65AF1-E2EB-444B-BA24-4ADCE89D2810}">
   <dimension ref="A1:F22"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="A7" sqref="A7:A22"/>
     </sheetView>
   </sheetViews>
@@ -2547,7 +2544,7 @@
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B3">
         <v>90</v>
@@ -2627,7 +2624,7 @@
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B7">
         <v>90</v>
@@ -2887,7 +2884,7 @@
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B20">
         <v>90</v>
@@ -2907,7 +2904,7 @@
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B21">
         <v>90</v>
@@ -2927,7 +2924,7 @@
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B22">
         <v>90</v>
@@ -3002,7 +2999,7 @@
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B3">
         <v>85</v>
@@ -3082,7 +3079,7 @@
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B7">
         <v>85</v>
@@ -3342,7 +3339,7 @@
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B20">
         <v>85</v>
@@ -3362,7 +3359,7 @@
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B21">
         <v>85</v>
@@ -3382,7 +3379,7 @@
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B22">
         <v>85</v>
@@ -3409,8 +3406,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7395B4B6-3B03-44E2-AB59-41FE5E2B4293}">
   <dimension ref="A1:C14"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C17" sqref="C17"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="O13" sqref="O13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3425,7 +3422,7 @@
         <v>22</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>23</v>
+        <v>29</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
@@ -3433,11 +3430,11 @@
         <f>cond_exp!A10</f>
         <v>Competition</v>
       </c>
-      <c r="B2" s="3">
+      <c r="B2" s="4">
         <f>cond_exp!C10</f>
         <v>0.64444444444444404</v>
       </c>
-      <c r="C2" s="3">
+      <c r="C2" s="4">
         <f>cond_ctr!C10</f>
         <v>0.152941176470588</v>
       </c>
@@ -3447,11 +3444,11 @@
         <f>cond_exp!A11</f>
         <v>Completion</v>
       </c>
-      <c r="B3" s="3">
+      <c r="B3" s="4">
         <f>cond_exp!C11</f>
         <v>0.62222222222222201</v>
       </c>
-      <c r="C3" s="3">
+      <c r="C3" s="4">
         <f>cond_ctr!C11</f>
         <v>0.21176470588235199</v>
       </c>
@@ -3461,11 +3458,11 @@
         <f>cond_exp!A9</f>
         <v>Challenge</v>
       </c>
-      <c r="B4" s="3">
+      <c r="B4" s="4">
         <f>cond_exp!C9</f>
         <v>0.78888888888888797</v>
       </c>
-      <c r="C4" s="3">
+      <c r="C4" s="4">
         <f>cond_ctr!C9</f>
         <v>0.34117647058823503</v>
       </c>
@@ -3475,11 +3472,11 @@
         <f>cond_exp!A16</f>
         <v>Humor</v>
       </c>
-      <c r="B5" s="3">
+      <c r="B5" s="4">
         <f>cond_exp!C16</f>
         <v>0.27777777777777701</v>
       </c>
-      <c r="C5" s="3">
+      <c r="C5" s="4">
         <f>cond_ctr!C16</f>
         <v>0.35294117647058798</v>
       </c>
@@ -3489,11 +3486,11 @@
         <f>cond_exp!A18</f>
         <v>Relaxation</v>
       </c>
-      <c r="B6" s="3">
+      <c r="B6" s="4">
         <f>cond_exp!C18</f>
         <v>0.51111111111111096</v>
       </c>
-      <c r="C6" s="3">
+      <c r="C6" s="4">
         <f>cond_ctr!C18</f>
         <v>0.35294117647058798</v>
       </c>
@@ -3503,11 +3500,11 @@
         <f>cond_exp!A17</f>
         <v>Nurture</v>
       </c>
-      <c r="B7" s="3">
+      <c r="B7" s="4">
         <f>cond_exp!C17</f>
         <v>0.46666666666666601</v>
       </c>
-      <c r="C7" s="3">
+      <c r="C7" s="4">
         <f>cond_ctr!C17</f>
         <v>0.48235294117646998</v>
       </c>
@@ -3517,11 +3514,11 @@
         <f>cond_exp!A8</f>
         <v>Captivation</v>
       </c>
-      <c r="B8" s="3">
+      <c r="B8" s="4">
         <f>cond_exp!C8</f>
         <v>0.58888888888888802</v>
       </c>
-      <c r="C8" s="3">
+      <c r="C8" s="4">
         <f>cond_ctr!C8</f>
         <v>0.494117647058823</v>
       </c>
@@ -3531,11 +3528,11 @@
         <f>cond_exp!A13</f>
         <v>Progression</v>
       </c>
-      <c r="B9" s="3">
+      <c r="B9" s="4">
         <f>cond_exp!C13</f>
         <v>0.74444444444444402</v>
       </c>
-      <c r="C9" s="3">
+      <c r="C9" s="4">
         <f>cond_ctr!C13</f>
         <v>0.50588235294117601</v>
       </c>
@@ -3545,11 +3542,11 @@
         <f>cond_exp!A15</f>
         <v>Fantasy</v>
       </c>
-      <c r="B10" s="3">
+      <c r="B10" s="4">
         <f>cond_exp!C15</f>
         <v>0.688888888888888</v>
       </c>
-      <c r="C10" s="3">
+      <c r="C10" s="4">
         <f>cond_ctr!C15</f>
         <v>0.51764705882352902</v>
       </c>
@@ -3559,11 +3556,11 @@
         <f>cond_exp!A19</f>
         <v>Sensation</v>
       </c>
-      <c r="B11" s="3">
+      <c r="B11" s="4">
         <f>cond_exp!C19</f>
         <v>0.688888888888888</v>
       </c>
-      <c r="C11" s="3">
+      <c r="C11" s="4">
         <f>cond_ctr!C19</f>
         <v>0.51764705882352902</v>
       </c>
@@ -3573,11 +3570,11 @@
         <f>cond_exp!A12</f>
         <v>Discovery</v>
       </c>
-      <c r="B12" s="3">
+      <c r="B12" s="4">
         <f>cond_exp!C12</f>
         <v>0.76666666666666605</v>
       </c>
-      <c r="C12" s="3">
+      <c r="C12" s="4">
         <f>cond_ctr!C12</f>
         <v>0.78823529411764703</v>
       </c>
@@ -3587,11 +3584,11 @@
         <f>cond_exp!A14</f>
         <v>Exploration</v>
       </c>
-      <c r="B13" s="3">
+      <c r="B13" s="4">
         <f>cond_exp!C14</f>
         <v>0.95555555555555505</v>
       </c>
-      <c r="C13" s="3">
+      <c r="C13" s="4">
         <f>cond_ctr!C14</f>
         <v>0.90588235294117603</v>
       </c>
@@ -3639,12 +3636,12 @@
         <v>22</v>
       </c>
       <c r="C1" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B2" s="1">
         <v>17.336165000000001</v>
@@ -3677,7 +3674,7 @@
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B5" s="1">
         <v>7.74444444444444</v>
@@ -3820,7 +3817,7 @@
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B18" s="1">
         <v>0.10307401156550999</v>
@@ -3831,7 +3828,7 @@
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B19" s="1">
         <v>17.419282222222201</v>
@@ -3842,7 +3839,7 @@
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B20" s="1">
         <v>2.88627066292736E-2</v>

</xml_diff>